<commit_message>
Version2.5 modified schematic and code updated
</commit_message>
<xml_diff>
--- a/Projects/tractor/input/LOGIC TABLE.xlsx
+++ b/Projects/tractor/input/LOGIC TABLE.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8DE5A3-51EA-4F8D-9A6C-8F48F81EA122}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -290,15 +291,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -311,6 +303,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,6 +406,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -440,6 +458,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -615,12 +650,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="topRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,40 +669,42 @@
     <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.7109375" customWidth="1"/>
+    <col min="10" max="10" width="55" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -699,7 +736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -730,11 +767,23 @@
       <c r="J4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -765,11 +814,23 @@
       <c r="J5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -800,8 +861,23 @@
       <c r="J6" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -826,8 +902,23 @@
       <c r="H7" s="7"/>
       <c r="I7" s="10"/>
       <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -856,8 +947,23 @@
         <v>10</v>
       </c>
       <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -886,8 +992,23 @@
       <c r="J9" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -916,38 +1037,68 @@
         <v>10</v>
       </c>
       <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <v>8</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="21" t="s">
+      <c r="B11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="20" t="s">
+      <c r="F11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="20">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" s="20">
+        <v>1</v>
+      </c>
+      <c r="O11" s="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -978,8 +1129,23 @@
       <c r="J12" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -1010,8 +1176,20 @@
       <c r="J13" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -1042,8 +1220,23 @@
       <c r="J14" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -1074,8 +1267,23 @@
       <c r="J15" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -1104,8 +1312,20 @@
         <v>10</v>
       </c>
       <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1116,15 +1336,27 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="24" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -1133,13 +1365,28 @@
       <c r="J18" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
       <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="5" t="s">
         <v>33</v>
       </c>
@@ -1150,62 +1397,312 @@
       <c r="J19" t="s">
         <v>30</v>
       </c>
-      <c r="K19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19" s="20">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" s="20">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="19"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="5"/>
       <c r="H20" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
+    <row r="21" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="24"/>
       <c r="C21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="19"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="5"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
       <c r="B24" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1224,7 +1721,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1236,7 +1733,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>